<commit_message>
* Added via stiching* Added via stiching* Added via stiching* Added via stiching* Added via stiching* Added via stiching* Added via stiching* Added via stiching* Added via stiching
</commit_message>
<xml_diff>
--- a/MIXR User Interface/Project Outputs for MIXR User Interface/MIXR User Interface_1.0.xlsx
+++ b/MIXR User Interface/Project Outputs for MIXR User Interface/MIXR User Interface_1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taiping\Documents\FYDP\mixr-hardware\MIXR User Interface\Project Outputs for MIXR User Interface\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D78DC95E-5A2A-41E4-92AB-250B6CB05913}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C282B53A-68EC-49B2-BCE0-C20A4B8CF7CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3045" yWindow="3780" windowWidth="28800" windowHeight="8220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,7 +111,7 @@
     <t>Taiping Li</t>
   </si>
   <si>
-    <t>2020-02-08 10:12 PM</t>
+    <t>2020-02-09 9:09 PM</t>
   </si>
   <si>
     <t>1</t>
@@ -399,10 +399,10 @@
     <t>Bill of Materials for Project [MIXR User Interface.PrjPcb] (No PCB Document Selected)</t>
   </si>
   <si>
-    <t>10:12 PM</t>
-  </si>
-  <si>
-    <t>2020-02-08</t>
+    <t>9:09 PM</t>
+  </si>
+  <si>
+    <t>2020-02-09</t>
   </si>
   <si>
     <t>BOM_PartType</t>

</xml_diff>